<commit_message>
Doc: Updated Indicators sheet
</commit_message>
<xml_diff>
--- a/Project Management Plan/Indicators.xlsx
+++ b/Project Management Plan/Indicators.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Project Management Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEFE460A-9301-477C-BB80-751D7777CE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C74A5E4-AD86-4D47-8C0C-F29EBD098DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,15 +25,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>CRS</t>
+    <t>Total CRS</t>
   </si>
   <si>
-    <t>SRS</t>
+    <t>Total SRS</t>
   </si>
   <si>
-    <t>TC</t>
+    <t>Total TC</t>
+  </si>
+  <si>
+    <t>Total TC
+Executed</t>
+  </si>
+  <si>
+    <t>Total TC
+Passed</t>
+  </si>
+  <si>
+    <t>Total TC 
+Failed</t>
   </si>
 </sst>
 </file>
@@ -97,13 +109,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -385,124 +400,232 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="1">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="2">
         <v>30</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="1">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="2">
         <v>54</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="1">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="2">
         <v>82</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="12">
+    <mergeCell ref="A13:C16"/>
+    <mergeCell ref="D13:F16"/>
+    <mergeCell ref="A17:C20"/>
+    <mergeCell ref="D17:F20"/>
+    <mergeCell ref="A21:C24"/>
+    <mergeCell ref="D21:F24"/>
     <mergeCell ref="A1:C4"/>
     <mergeCell ref="A5:C8"/>
     <mergeCell ref="A9:C12"/>

</xml_diff>

<commit_message>
Doc: updated Indicators sheet with failed test cases
</commit_message>
<xml_diff>
--- a/Project Management Plan/Indicators.xlsx
+++ b/Project Management Plan/Indicators.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Project Management Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C99CB00-4D0C-4A2B-9605-3335511A0516}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ED7836-C81D-486B-B68E-95AAEB50B472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -406,8 +417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J22" sqref="J22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,7 +574,7 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -599,7 +610,7 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>

</xml_diff>

<commit_message>
Doc: Updated Indicators sheet for test cases after fixes
</commit_message>
<xml_diff>
--- a/Project Management Plan/Indicators.xlsx
+++ b/Project Management Plan/Indicators.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\QA\Online-Mobile-Store-WebSite\Project Management Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02ED7836-C81D-486B-B68E-95AAEB50B472}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81901D37-BF6B-4BF0-AF8E-4E711D14A723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,7 +418,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="D21" sqref="D21:F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -574,7 +574,7 @@
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="3">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -610,7 +610,7 @@
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="3">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>

</xml_diff>